<commit_message>
Screenshot is saved in same folder as the report and working fine
</commit_message>
<xml_diff>
--- a/test_cases/New Microsoft Excel Worksheet.xlsx
+++ b/test_cases/New Microsoft Excel Worksheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BhartiPr\PycharmProjects\SalesforceDemo\test_cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ADEC566-E321-4875-8E6F-FB5F54ABF09C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{119AA7FF-5A9C-4465-8B06-96A5DAE109D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="57">
   <si>
     <t>Test ID</t>
   </si>
@@ -193,6 +193,9 @@
   </si>
   <si>
     <t xml:space="preserve">Fail a Opportunity </t>
+  </si>
+  <si>
+    <t>click Opportunity record with value="Tryedit"</t>
   </si>
 </sst>
 </file>
@@ -521,13 +524,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -583,7 +586,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:18" ht="105" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>48</v>
       </c>
@@ -621,7 +624,7 @@
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
     </row>
-    <row r="3" spans="1:18" ht="116" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:18" ht="135" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>49</v>
       </c>
@@ -677,7 +680,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="116" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:18" ht="120" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>50</v>
       </c>
@@ -706,7 +709,7 @@
         <v>31</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>42</v>
@@ -723,7 +726,7 @@
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
     </row>
-    <row r="5" spans="1:18" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:18" ht="105" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>51</v>
       </c>
@@ -752,7 +755,7 @@
         <v>31</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>42</v>
@@ -767,7 +770,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:18" ht="105" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>52</v>
       </c>

</xml_diff>